<commit_message>
ejemplos arrays + ordenacion ranking adivina parejas
</commit_message>
<xml_diff>
--- a/Keyboard Shortcuts.xlsx
+++ b/Keyboard Shortcuts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\20180423 - Formación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\20180423 - Formación\20180513 - Curso JS-Ionic\coursejs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>Indentar el código</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>Buscar todas las referencias</t>
+  </si>
+  <si>
+    <t>Tool</t>
+  </si>
+  <si>
+    <t>Comando</t>
   </si>
 </sst>
 </file>
@@ -430,8 +436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D6:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,6 +449,12 @@
   </cols>
   <sheetData>
     <row r="6" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
       <c r="F6" t="s">
         <v>3</v>
       </c>
@@ -452,16 +464,13 @@
     </row>
     <row r="7" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="4:7" x14ac:dyDescent="0.25">
@@ -469,13 +478,13 @@
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.25">
@@ -483,24 +492,27 @@
         <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="G10" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="4:7" x14ac:dyDescent="0.25">

</xml_diff>